<commit_message>
change EDA to excel file
</commit_message>
<xml_diff>
--- a/screening_deep_sitee.xlsx
+++ b/screening_deep_sitee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ΔΗΜΗΤΡΗΣ\Documents\GitHubs\AI-marine-litter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE6062C-3F5F-4123-B0A3-3A1BB831145E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B5B559-9996-4C1D-844D-D4392A060DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30075" yWindow="330" windowWidth="25665" windowHeight="13320" xr2:uid="{9E4A43DE-8FF9-4A91-B492-0B4C1599A160}"/>
+    <workbookView xWindow="31980" yWindow="1485" windowWidth="23295" windowHeight="11055" xr2:uid="{9E4A43DE-8FF9-4A91-B492-0B4C1599A160}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -531,9 +531,6 @@
     <t>Sem-Seg</t>
   </si>
   <si>
-    <t>EDA</t>
-  </si>
-  <si>
     <t>Classification, Detection, Instance segmentation</t>
   </si>
   <si>
@@ -625,6 +622,9 @@
   </si>
   <si>
     <t>Dataset access</t>
+  </si>
+  <si>
+    <t>ED</t>
   </si>
 </sst>
 </file>
@@ -1153,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789D46A0-4CC3-42C0-9023-C48815470A65}">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1196,19 +1196,19 @@
         <v>144</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>186</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>187</v>
       </c>
       <c r="J1" s="17" t="s">
         <v>146</v>
       </c>
       <c r="K1" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>184</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1237,7 +1237,7 @@
         <v>145</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>147</v>
@@ -1267,10 +1267,10 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>143</v>
@@ -1279,7 +1279,7 @@
         <v>148</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>141</v>
@@ -1290,28 +1290,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C4" s="4">
         <v>2022</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>88</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>149</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>148</v>
@@ -1328,28 +1328,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" s="4">
         <v>2022</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>86</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>149</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>148</v>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>145</v>
@@ -1423,7 +1423,7 @@
         <v>149</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>148</v>
@@ -1461,7 +1461,7 @@
         <v>145</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>148</v>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>145</v>
@@ -1529,13 +1529,13 @@
         <v>98</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>145</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>147</v>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>145</v>
@@ -1577,7 +1577,7 @@
         <v>148</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L11" s="7" t="s">
         <v>141</v>
@@ -1609,7 +1609,7 @@
         <v>149</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>148</v>
@@ -1647,13 +1647,13 @@
         <v>149</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>148</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L13" s="7" t="s">
         <v>83</v>
@@ -1685,13 +1685,13 @@
         <v>145</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>148</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L14" s="7" t="s">
         <v>142</v>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>145</v>
@@ -1727,7 +1727,7 @@
         <v>148</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>141</v>
@@ -1753,13 +1753,13 @@
         <v>86</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>145</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>147</v>
@@ -1797,7 +1797,7 @@
         <v>149</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>147</v>
@@ -1835,13 +1835,13 @@
         <v>149</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>147</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L18" s="7" t="s">
         <v>142</v>
@@ -1873,13 +1873,13 @@
         <v>145</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>148</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L19" s="7" t="s">
         <v>155</v>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>145</v>
@@ -1918,7 +1918,7 @@
         <v>82</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1939,7 +1939,7 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>145</v>
@@ -1951,10 +1951,10 @@
         <v>148</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -1977,19 +1977,19 @@
         <v>92</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>149</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>148</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L22" s="7" t="s">
         <v>155</v>
@@ -2000,34 +2000,34 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23" s="4">
         <v>2022</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="F23" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>81</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>147</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L23" s="7" t="s">
         <v>142</v>
@@ -2059,13 +2059,13 @@
         <v>149</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J24" s="8" t="s">
         <v>148</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L24" s="7" t="s">
         <v>140</v>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="F25" s="27"/>
       <c r="G25" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H25" s="24" t="s">
         <v>145</v>
@@ -2101,10 +2101,10 @@
         <v>148</v>
       </c>
       <c r="K25" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L25" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>145</v>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>145</v>
@@ -2209,7 +2209,7 @@
         <v>148</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>141</v>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>145</v>
@@ -2245,7 +2245,7 @@
         <v>148</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L29" s="7" t="s">
         <v>141</v>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>145</v>
@@ -2313,7 +2313,7 @@
         <v>149</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>148</v>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H32" s="24" t="s">
         <v>145</v>
@@ -2358,7 +2358,7 @@
         <v>154</v>
       </c>
       <c r="L32" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>145</v>
@@ -2391,7 +2391,7 @@
         <v>148</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L33" s="7" t="s">
         <v>141</v>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>145</v>
@@ -2427,7 +2427,7 @@
         <v>148</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>141</v>
@@ -2459,7 +2459,7 @@
         <v>145</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J35" s="8" t="s">
         <v>147</v>
@@ -2497,7 +2497,7 @@
         <v>149</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>147</v>
@@ -2529,19 +2529,19 @@
         <v>96</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>145</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>148</v>
       </c>
       <c r="K37" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L37" s="7" t="s">
         <v>141</v>
@@ -2573,13 +2573,13 @@
         <v>145</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J38" s="8" t="s">
         <v>148</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L38" s="7" t="s">
         <v>141</v>
@@ -2590,16 +2590,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C39" s="4">
         <v>2022</v>
       </c>
       <c r="D39" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="F39" s="11" t="s">
         <v>93</v>
@@ -2611,10 +2611,10 @@
         <v>145</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L39" s="7" t="s">
         <v>141</v>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>145</v>
@@ -2674,10 +2674,10 @@
       </c>
       <c r="F41" s="33"/>
       <c r="G41" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I41" s="34" t="s">
         <v>143</v>
@@ -2686,7 +2686,7 @@
         <v>148</v>
       </c>
       <c r="K41" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L41" s="20" t="s">
         <v>141</v>
@@ -2712,19 +2712,19 @@
         <v>94</v>
       </c>
       <c r="G42" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H42" s="31" t="s">
         <v>145</v>
       </c>
       <c r="I42" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J42" s="37" t="s">
         <v>148</v>
       </c>
       <c r="K42" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L42" s="22" t="s">
         <v>141</v>
@@ -2750,13 +2750,13 @@
         <v>93</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>145</v>
       </c>
       <c r="I43" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J43" s="37" t="s">
         <v>148</v>
@@ -2788,13 +2788,13 @@
         <v>99</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>145</v>
       </c>
       <c r="I44" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J44" s="37" t="s">
         <v>148</v>
@@ -2824,7 +2824,7 @@
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H45" s="12" t="s">
         <v>145</v>

</xml_diff>